<commit_message>
chore: hospitais do nivel quaternario
</commit_message>
<xml_diff>
--- a/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
+++ b/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D159" sqref="D155:D159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chore: actualizacao de centro de saude e posto de saude
</commit_message>
<xml_diff>
--- a/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
+++ b/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="106">
   <si>
     <t>Nivel</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Hospitais Distritais</t>
-  </si>
-  <si>
-    <t>Hospitais Ruraus</t>
   </si>
   <si>
     <t>Hospitais Gerais</t>
@@ -192,9 +189,6 @@
     <t>Centro de Saude Matola-Gare</t>
   </si>
   <si>
-    <t>Centro de Saude Muhalaze</t>
-  </si>
-  <si>
     <t>Centro de Saude Ndlavela</t>
   </si>
   <si>
@@ -265,13 +259,97 @@
   </si>
   <si>
     <t>Cidade de Maputo, KaMubukwana</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Mutsekua</t>
+  </si>
+  <si>
+    <t>Hospitais Rurais</t>
+  </si>
+  <si>
+    <t>Centro de Saude Eduardo Mondlane</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Marracuene</t>
+  </si>
+  <si>
+    <t>Marracuene</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Mualaze</t>
+  </si>
+  <si>
+    <t>Centro de Saude da Manhica</t>
+  </si>
+  <si>
+    <t>Manhica</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Magude</t>
+  </si>
+  <si>
+    <t>Posto de Saude da Mozal</t>
+  </si>
+  <si>
+    <t>Centro de Saude da Moamba</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Mali</t>
+  </si>
+  <si>
+    <t>Cidade da Matola</t>
+  </si>
+  <si>
+    <t>Centro de Saude Massaca II</t>
+  </si>
+  <si>
+    <t>Boane</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Tsalala</t>
+  </si>
+  <si>
+    <t>Tsalala</t>
+  </si>
+  <si>
+    <t>Centro de Saude Massaca</t>
+  </si>
+  <si>
+    <t>Zitundo</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Machubo</t>
+  </si>
+  <si>
+    <t>Machubo</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Namaacha</t>
+  </si>
+  <si>
+    <t>Namaacha</t>
+  </si>
+  <si>
+    <t>Magude</t>
+  </si>
+  <si>
+    <t>Centro de Saude da Ponta de Ouro</t>
+  </si>
+  <si>
+    <t>Centro de Saude do Fomento</t>
+  </si>
+  <si>
+    <t>Cidade da Matola, Fomento</t>
+  </si>
+  <si>
+    <t>Cidade de Maputo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +368,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Garamond"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -312,10 +395,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +720,7 @@
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -658,7 +744,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -679,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -703,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -727,10 +813,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="2">
         <v>-25.938320000000001</v>
@@ -757,10 +843,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="2">
         <v>-25.96011</v>
@@ -787,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -811,10 +897,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="2">
         <v>-25.9742</v>
@@ -841,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -865,10 +951,10 @@
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F9" s="2">
         <v>-25.916350000000001</v>
@@ -895,10 +981,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="2">
         <v>-25.897210000000001</v>
@@ -925,10 +1011,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2">
         <v>-25.831219999999998</v>
@@ -955,10 +1041,10 @@
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F12" s="2">
         <v>-25.84639</v>
@@ -985,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1009,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1033,7 +1119,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1057,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1081,11 +1167,17 @@
         <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-25.927630000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>32.594659999999998</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1105,10 +1197,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F18" s="2">
         <v>-25.842289999999998</v>
@@ -1135,10 +1227,10 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19" s="2">
         <v>-25.915120000000002</v>
@@ -1165,10 +1257,10 @@
         <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F20" s="2">
         <v>-25.872140000000002</v>
@@ -1195,10 +1287,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F21" s="2">
         <v>-25.905760000000001</v>
@@ -1225,9 +1317,11 @@
         <v>5</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="F22" s="2">
         <v>-25.914400000000001</v>
       </c>
@@ -1253,10 +1347,10 @@
         <v>5</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="2">
         <v>-25.950939999999999</v>
@@ -1283,10 +1377,10 @@
         <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F24" s="2">
         <v>-26.00329</v>
@@ -1313,10 +1407,10 @@
         <v>5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2">
         <v>-26.023140000000001</v>
@@ -1343,10 +1437,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2">
         <v>-25.73921</v>
@@ -1373,7 +1467,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2">
@@ -1401,7 +1495,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1425,7 +1519,7 @@
         <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1449,7 +1543,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1473,7 +1567,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1497,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1521,7 +1615,7 @@
         <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1545,7 +1639,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1569,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1593,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1617,7 +1711,7 @@
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1640,9 +1734,7 @@
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1665,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1689,7 +1781,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1713,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1737,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1760,10 +1852,18 @@
       <c r="C43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="D43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="2">
+        <v>-26.011081000000001</v>
+      </c>
+      <c r="G43" s="2">
+        <v>32.567492000000001</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -1782,10 +1882,18 @@
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="D44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="2">
+        <v>-25.731567600000002</v>
+      </c>
+      <c r="G44" s="2">
+        <v>32.670907100000001</v>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -1804,10 +1912,18 @@
       <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F45" s="2">
+        <v>-25.653556500000001</v>
+      </c>
+      <c r="G45" s="2">
+        <v>32.672116799999998</v>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -1826,10 +1942,18 @@
       <c r="C46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="2">
+        <v>-25.776476899999999</v>
+      </c>
+      <c r="G46" s="2">
+        <v>32.5183781</v>
+      </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -1848,10 +1972,18 @@
       <c r="C47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="2">
+        <v>-25.40767</v>
+      </c>
+      <c r="G47" s="2">
+        <v>32.80724</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -1870,10 +2002,18 @@
       <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="2">
+        <v>-25.028939999999999</v>
+      </c>
+      <c r="G48" s="2">
+        <v>32.648989999999998</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -1892,10 +2032,16 @@
       <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="F49" s="2">
+        <v>-25.598739999999999</v>
+      </c>
+      <c r="G49" s="2">
+        <v>32.244964000000003</v>
+      </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -1914,10 +2060,18 @@
       <c r="C50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" s="2">
+        <v>-25.761462000000002</v>
+      </c>
+      <c r="G50" s="2">
+        <v>32.568606000000003</v>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -1936,10 +2090,18 @@
       <c r="C51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F51" s="2">
+        <v>-26.064394</v>
+      </c>
+      <c r="G51" s="2">
+        <v>32.286631999999997</v>
+      </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -1958,10 +2120,18 @@
       <c r="C52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F52" s="3">
+        <v>-25.894861649885499</v>
+      </c>
+      <c r="G52" s="3">
+        <v>32.4616652727127</v>
+      </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -1980,10 +2150,18 @@
       <c r="C53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F53" s="2">
+        <v>-26.064789999999999</v>
+      </c>
+      <c r="G53" s="2">
+        <v>32.286414999999998</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2002,10 +2180,18 @@
       <c r="C54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="2">
+        <v>-26.837185999999999</v>
+      </c>
+      <c r="G54" s="2">
+        <v>32.884238000000003</v>
+      </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2024,10 +2210,18 @@
       <c r="C55" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" s="2">
+        <v>-25.564392999999999</v>
+      </c>
+      <c r="G55" s="2">
+        <v>32.799444999999999</v>
+      </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2046,10 +2240,18 @@
       <c r="C56" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="2">
+        <v>-25.991039000000001</v>
+      </c>
+      <c r="G56" s="2">
+        <v>32.132820000000002</v>
+      </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -2068,10 +2270,18 @@
       <c r="C57" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="2">
+        <v>-25.934336900000002</v>
+      </c>
+      <c r="G57" s="2">
+        <v>32.4761886</v>
+      </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -3763,7 +3973,7 @@
         <v>7</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
@@ -3787,7 +3997,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -3810,10 +4020,16 @@
       <c r="C136" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D136" s="2"/>
+      <c r="D136" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
+      <c r="F136" s="2">
+        <v>-25.918668499999999</v>
+      </c>
+      <c r="G136" s="2">
+        <v>32.394661399999997</v>
+      </c>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
@@ -4204,7 +4420,7 @@
         <v>9</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -4226,10 +4442,10 @@
         <v>9</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E155" s="2"/>
       <c r="F155" s="2">
@@ -4254,14 +4470,18 @@
         <v>9</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-      <c r="G156" s="2"/>
+      <c r="F156" s="3">
+        <v>-25.947144000000002</v>
+      </c>
+      <c r="G156" s="3">
+        <v>32.543959999999998</v>
+      </c>
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
       <c r="J156" s="2"/>
@@ -4278,14 +4498,18 @@
         <v>9</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
+      <c r="F157" s="2">
+        <v>-25.951118999999998</v>
+      </c>
+      <c r="G157" s="2">
+        <v>32.555467999999998</v>
+      </c>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
       <c r="J157" s="2"/>
@@ -4302,14 +4526,18 @@
         <v>9</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
-      <c r="G158" s="2"/>
+      <c r="F158" s="2">
+        <v>-25.935561</v>
+      </c>
+      <c r="G158" s="3">
+        <v>32.611508999999998</v>
+      </c>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
       <c r="J158" s="2"/>
@@ -4326,10 +4554,10 @@
         <v>9</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" s="2">
@@ -4351,13 +4579,13 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D160" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E160" s="2"/>
       <c r="F160" s="2">
@@ -4379,13 +4607,13 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D161" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E161" s="2"/>
       <c r="F161" s="2">
@@ -4407,17 +4635,21 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
-      <c r="G162" s="2"/>
+      <c r="F162" s="2">
+        <v>-25.859612800000001</v>
+      </c>
+      <c r="G162" s="2">
+        <v>32.566635499999997</v>
+      </c>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
       <c r="J162" s="2"/>
@@ -4431,13 +4663,13 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E163" s="2"/>
       <c r="F163" s="2">

</xml_diff>

<commit_message>
chore: actualizacao do relatorio
</commit_message>
<xml_diff>
--- a/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
+++ b/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="109">
   <si>
     <t>Nivel</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Centro de Saude Sao Damaso</t>
   </si>
   <si>
-    <t>Centro de Saude Tsalala</t>
-  </si>
-  <si>
     <t>Centro de Saude Unidade A</t>
   </si>
   <si>
@@ -343,6 +340,18 @@
   </si>
   <si>
     <t>Cidade de Maputo</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Maluana</t>
+  </si>
+  <si>
+    <t>Maluana</t>
+  </si>
+  <si>
+    <t>Hospital Distrital de Manhica</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Maragra</t>
   </si>
 </sst>
 </file>
@@ -710,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +729,7 @@
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -744,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -816,7 +825,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="2">
         <v>-25.938320000000001</v>
@@ -846,7 +855,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="2">
         <v>-25.96011</v>
@@ -900,7 +909,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="2">
         <v>-25.9742</v>
@@ -954,7 +963,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" s="2">
         <v>-25.916350000000001</v>
@@ -984,7 +993,7 @@
         <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2">
         <v>-25.897210000000001</v>
@@ -1014,7 +1023,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2">
         <v>-25.831219999999998</v>
@@ -1044,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="2">
         <v>-25.84639</v>
@@ -1121,9 +1130,15 @@
       <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="3">
+        <v>-25.948110967492099</v>
+      </c>
+      <c r="G15" s="3">
+        <v>32.589699178934097</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1170,7 +1185,7 @@
         <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F17" s="2">
         <v>-25.927630000000001</v>
@@ -1200,7 +1215,7 @@
         <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="2">
         <v>-25.842289999999998</v>
@@ -1230,7 +1245,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="2">
         <v>-25.915120000000002</v>
@@ -1260,7 +1275,7 @@
         <v>36</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="2">
         <v>-25.872140000000002</v>
@@ -1290,7 +1305,7 @@
         <v>37</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="2">
         <v>-25.905760000000001</v>
@@ -1320,7 +1335,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="2">
         <v>-25.914400000000001</v>
@@ -1350,7 +1365,7 @@
         <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="2">
         <v>-25.950939999999999</v>
@@ -1380,7 +1395,7 @@
         <v>39</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2">
         <v>-26.00329</v>
@@ -1410,7 +1425,7 @@
         <v>41</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" s="2">
         <v>-26.023140000000001</v>
@@ -1440,7 +1455,7 @@
         <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="2">
         <v>-25.73921</v>
@@ -1469,7 +1484,9 @@
       <c r="D27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="F27" s="2">
         <v>-25.966349999999998</v>
       </c>
@@ -1734,10 +1751,18 @@
       <c r="C38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="3">
+        <v>-25.496123350534798</v>
+      </c>
+      <c r="G38" s="3">
+        <v>32.652332782745297</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1804,9 +1829,7 @@
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1829,7 +1852,7 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1853,10 +1876,10 @@
         <v>5</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F43" s="2">
         <v>-26.011081000000001</v>
@@ -1883,10 +1906,10 @@
         <v>5</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="F44" s="2">
         <v>-25.731567600000002</v>
@@ -1913,10 +1936,10 @@
         <v>5</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F45" s="2">
         <v>-25.653556500000001</v>
@@ -1943,10 +1966,10 @@
         <v>5</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F46" s="2">
         <v>-25.776476899999999</v>
@@ -1973,16 +1996,16 @@
         <v>5</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F47" s="2">
-        <v>-25.40767</v>
+        <v>-25.409322476996099</v>
       </c>
       <c r="G47" s="2">
-        <v>32.80724</v>
+        <v>32.807678282260902</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -2003,10 +2026,10 @@
         <v>5</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2">
         <v>-25.028939999999999</v>
@@ -2033,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2">
@@ -2061,10 +2084,10 @@
         <v>5</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="F50" s="2">
         <v>-25.761462000000002</v>
@@ -2091,10 +2114,10 @@
         <v>5</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="F51" s="2">
         <v>-26.064394</v>
@@ -2121,10 +2144,10 @@
         <v>5</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="F52" s="3">
         <v>-25.894861649885499</v>
@@ -2151,10 +2174,10 @@
         <v>5</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F53" s="2">
         <v>-26.064789999999999</v>
@@ -2181,10 +2204,10 @@
         <v>5</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F54" s="2">
         <v>-26.837185999999999</v>
@@ -2211,10 +2234,10 @@
         <v>5</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F55" s="2">
         <v>-25.564392999999999</v>
@@ -2241,10 +2264,10 @@
         <v>5</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="F56" s="2">
         <v>-25.991039000000001</v>
@@ -2271,10 +2294,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F57" s="2">
         <v>-25.934336900000002</v>
@@ -2300,10 +2323,16 @@
       <c r="C58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
+      <c r="F58" s="3">
+        <v>-25.457423632678498</v>
+      </c>
+      <c r="G58" s="3">
+        <v>32.772655338048899</v>
+      </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -3973,7 +4002,7 @@
         <v>7</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
@@ -3997,7 +4026,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -4021,7 +4050,7 @@
         <v>7</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2">
@@ -4400,10 +4429,18 @@
       <c r="C153" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
-      <c r="G153" s="2"/>
+      <c r="D153" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F153" s="3">
+        <v>-25.408708157686199</v>
+      </c>
+      <c r="G153" s="3">
+        <v>32.806573212146702</v>
+      </c>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
       <c r="J153" s="2"/>
@@ -4420,7 +4457,7 @@
         <v>9</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -4445,7 +4482,7 @@
         <v>11</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E155" s="2"/>
       <c r="F155" s="2">
@@ -4473,7 +4510,7 @@
         <v>11</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E156" s="2"/>
       <c r="F156" s="3">
@@ -4501,14 +4538,14 @@
         <v>11</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E157" s="2"/>
-      <c r="F157" s="2">
-        <v>-25.951118999999998</v>
+      <c r="F157" s="3">
+        <v>-25.951189612092001</v>
       </c>
       <c r="G157" s="2">
-        <v>32.555467999999998</v>
+        <v>32.555356174707399</v>
       </c>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
@@ -4529,7 +4566,7 @@
         <v>11</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E158" s="2"/>
       <c r="F158" s="2">
@@ -4557,7 +4594,7 @@
         <v>11</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" s="2">
@@ -4585,7 +4622,7 @@
         <v>13</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E160" s="2"/>
       <c r="F160" s="2">
@@ -4613,7 +4650,7 @@
         <v>15</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E161" s="2"/>
       <c r="F161" s="2">
@@ -4641,7 +4678,7 @@
         <v>16</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E162" s="2"/>
       <c r="F162" s="2">
@@ -4669,7 +4706,7 @@
         <v>17</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E163" s="2"/>
       <c r="F163" s="2">

</xml_diff>

<commit_message>
Update US Maputo Cidade e Maputo Pronvicia.xlsx
</commit_message>
<xml_diff>
--- a/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
+++ b/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="113">
   <si>
     <t>Nivel</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>Posto de Saude de Inhagoia "A"</t>
+  </si>
+  <si>
+    <t>Centro de Saude de Magoanine A</t>
+  </si>
+  <si>
+    <t>Magoanine</t>
+  </si>
+  <si>
+    <t> 32.578765153884895</t>
   </si>
 </sst>
 </file>
@@ -722,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +742,7 @@
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -1832,10 +1841,18 @@
       <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="3">
+        <v>-25.895386493702301</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>

</xml_diff>

<commit_message>
chore: actualizacao de posto e centros de saude
</commit_message>
<xml_diff>
--- a/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
+++ b/Relatorio/US Maputo Cidade e Maputo Pronvicia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="125">
   <si>
     <t>Nivel</t>
   </si>
@@ -364,6 +364,42 @@
   </si>
   <si>
     <t> 32.578765153884895</t>
+  </si>
+  <si>
+    <t>Centro de Saude Campoane</t>
+  </si>
+  <si>
+    <t>Maputo</t>
+  </si>
+  <si>
+    <t>Centro de Saude da PRM</t>
+  </si>
+  <si>
+    <t>Centro de Saude de CMC</t>
+  </si>
+  <si>
+    <t>Centro de Saude da Zona Verde</t>
+  </si>
+  <si>
+    <t>Posto de Saude Unidade A</t>
+  </si>
+  <si>
+    <t>Centro de Saude Mosaka</t>
+  </si>
+  <si>
+    <t>Centro de Saude Maluana</t>
+  </si>
+  <si>
+    <t>Posto de Saude da Zona Verde</t>
+  </si>
+  <si>
+    <t>Centro de Saude Clinica Majaque</t>
+  </si>
+  <si>
+    <t>Centro de Saude Moyo</t>
+  </si>
+  <si>
+    <t>Posto de Saude Agua de Maputo</t>
   </si>
 </sst>
 </file>
@@ -731,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,9 +932,15 @@
       <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-25.977115999999999</v>
+      </c>
+      <c r="G6" s="3">
+        <v>32.587299999999999</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1094,9 +1136,15 @@
       <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-25.854903400000001</v>
+      </c>
+      <c r="G13" s="3">
+        <v>32.598505299999999</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1118,9 +1166,15 @@
       <c r="D14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="3">
+        <v>-25.962990300000001</v>
+      </c>
+      <c r="G14" s="3">
+        <v>32.593655200000001</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1172,9 +1226,15 @@
       <c r="D16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="3">
+        <v>-25.9342732</v>
+      </c>
+      <c r="G16" s="3">
+        <v>32.604108099999998</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2371,10 +2431,18 @@
       <c r="C59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" s="3">
+        <v>-26.040270499999998</v>
+      </c>
+      <c r="G59" s="3">
+        <v>32.326588299999997</v>
+      </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -2393,10 +2461,18 @@
       <c r="C60" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F60" s="3">
+        <v>-25.970670999999999</v>
+      </c>
+      <c r="G60" s="3">
+        <v>32.578015000000001</v>
+      </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -2415,10 +2491,18 @@
       <c r="C61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F61" s="3">
+        <v>-25.842690399999999</v>
+      </c>
+      <c r="G61" s="3">
+        <v>32.623810499999998</v>
+      </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2437,10 +2521,16 @@
       <c r="C62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
+      <c r="F62" s="3">
+        <v>-25.873816099999999</v>
+      </c>
+      <c r="G62" s="3">
+        <v>32.558492000000001</v>
+      </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -2459,10 +2549,16 @@
       <c r="C63" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="F63" s="3">
+        <v>-25.884333252219999</v>
+      </c>
+      <c r="G63" s="3">
+        <v>32.620500326156602</v>
+      </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -2481,10 +2577,16 @@
       <c r="C64" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+      <c r="F64" s="3">
+        <v>-25.496123350534798</v>
+      </c>
+      <c r="G64" s="3">
+        <v>32.652332782745297</v>
+      </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -2503,10 +2605,16 @@
       <c r="C65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
+      <c r="F65" s="3">
+        <v>-25.901843400000001</v>
+      </c>
+      <c r="G65" s="3">
+        <v>32.533523299999999</v>
+      </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -2525,10 +2633,12 @@
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -4125,10 +4235,16 @@
       <c r="C138" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D138" s="2"/>
+      <c r="D138" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
+      <c r="F138" s="3">
+        <v>-25.910542800000002</v>
+      </c>
+      <c r="G138" s="3">
+        <v>32.516980699999998</v>
+      </c>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
@@ -4147,10 +4263,16 @@
       <c r="C139" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D139" s="2"/>
+      <c r="D139" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
+      <c r="F139" s="3">
+        <v>-25.885989299999999</v>
+      </c>
+      <c r="G139" s="3">
+        <v>32.547624999999996</v>
+      </c>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
       <c r="J139" s="2"/>
@@ -4169,10 +4291,16 @@
       <c r="C140" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D140" s="2"/>
+      <c r="D140" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
+      <c r="F140" s="3">
+        <v>-26.046877899999998</v>
+      </c>
+      <c r="G140" s="3">
+        <v>32.334543500000002</v>
+      </c>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>

</xml_diff>